<commit_message>
RLC metadata, don't lose it!
</commit_message>
<xml_diff>
--- a/photobiology/fvfm_07152024.xlsx
+++ b/photobiology/fvfm_07152024.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssdon\OneDrive\Documents\github\coral-leachate-heat\photobiology\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11617D3E-E116-4E2F-AA41-879C40353BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="16185" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -53,19 +59,201 @@
   </si>
   <si>
     <t>FO</t>
+  </si>
+  <si>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>H12C</t>
+  </si>
+  <si>
+    <t>H22C</t>
+  </si>
+  <si>
+    <t>H32C</t>
+  </si>
+  <si>
+    <t>H42C</t>
+  </si>
+  <si>
+    <t>H52C</t>
+  </si>
+  <si>
+    <t>H62C</t>
+  </si>
+  <si>
+    <t>H72C</t>
+  </si>
+  <si>
+    <t>H82C</t>
+  </si>
+  <si>
+    <t>H92C</t>
+  </si>
+  <si>
+    <t>H102C</t>
+  </si>
+  <si>
+    <t>H52H</t>
+  </si>
+  <si>
+    <t>H62H</t>
+  </si>
+  <si>
+    <t>H22H</t>
+  </si>
+  <si>
+    <t>H92H</t>
+  </si>
+  <si>
+    <t>H32H</t>
+  </si>
+  <si>
+    <t>H42L</t>
+  </si>
+  <si>
+    <t>H62L</t>
+  </si>
+  <si>
+    <t>H102L</t>
+  </si>
+  <si>
+    <t>H12L</t>
+  </si>
+  <si>
+    <t>H72L</t>
+  </si>
+  <si>
+    <t>A92C</t>
+  </si>
+  <si>
+    <t>A102C</t>
+  </si>
+  <si>
+    <t>A22C</t>
+  </si>
+  <si>
+    <t>A72C</t>
+  </si>
+  <si>
+    <t>A12C</t>
+  </si>
+  <si>
+    <t>A32L</t>
+  </si>
+  <si>
+    <t>A92L</t>
+  </si>
+  <si>
+    <t>A62L</t>
+  </si>
+  <si>
+    <t>A42L</t>
+  </si>
+  <si>
+    <t>A102L</t>
+  </si>
+  <si>
+    <t>A82H</t>
+  </si>
+  <si>
+    <t>A52H</t>
+  </si>
+  <si>
+    <t>A42H</t>
+  </si>
+  <si>
+    <t>A12H</t>
+  </si>
+  <si>
+    <t>A22H</t>
+  </si>
+  <si>
+    <t>A62C</t>
+  </si>
+  <si>
+    <t>H82H</t>
+  </si>
+  <si>
+    <t>H102H</t>
+  </si>
+  <si>
+    <t>H42H</t>
+  </si>
+  <si>
+    <t>H12H</t>
+  </si>
+  <si>
+    <t>H72H</t>
+  </si>
+  <si>
+    <t>H92L</t>
+  </si>
+  <si>
+    <t>H22L</t>
+  </si>
+  <si>
+    <t>H52L</t>
+  </si>
+  <si>
+    <t>H32L</t>
+  </si>
+  <si>
+    <t>H82L</t>
+  </si>
+  <si>
+    <t>A52L</t>
+  </si>
+  <si>
+    <t>A72L</t>
+  </si>
+  <si>
+    <t>A22L</t>
+  </si>
+  <si>
+    <t>A12L</t>
+  </si>
+  <si>
+    <t>A82L</t>
+  </si>
+  <si>
+    <t>A62H</t>
+  </si>
+  <si>
+    <t>A32H</t>
+  </si>
+  <si>
+    <t>A92H</t>
+  </si>
+  <si>
+    <t>A72H</t>
+  </si>
+  <si>
+    <t>A102H</t>
+  </si>
+  <si>
+    <t>A52C</t>
+  </si>
+  <si>
+    <t>A82C</t>
+  </si>
+  <si>
+    <t>A42C</t>
+  </si>
+  <si>
+    <t>A32C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="yy-mm-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="yy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss.000"/>
-    <numFmt numFmtId="166" formatCode="0"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,21 +286,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -150,7 +346,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -184,6 +380,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -218,9 +415,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -393,18 +591,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.73046875" customWidth="1"/>
+    <col min="2" max="2" width="13.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +632,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -444,12 +647,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
-        <v>45519.84418853009</v>
+        <v>45488.844189814816</v>
       </c>
       <c r="B3" s="2">
-        <v>45519.84418853009</v>
+        <v>45519.844188530093</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -470,12 +673,15 @@
         <v>915</v>
       </c>
       <c r="I3" s="4">
-        <v>0.668</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
-        <v>45519.84496263889</v>
+        <v>45488.844189814816</v>
       </c>
       <c r="B4" s="2">
         <v>45519.84496263889</v>
@@ -501,13 +707,16 @@
       <c r="I4" s="4">
         <v>0.621</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
-        <v>45519.84530517361</v>
+        <v>45488</v>
       </c>
       <c r="B5" s="2">
-        <v>45519.84530517361</v>
+        <v>45519.845305173607</v>
       </c>
       <c r="C5" s="3">
         <v>96478</v>
@@ -528,15 +737,18 @@
         <v>1630</v>
       </c>
       <c r="I5" s="4">
-        <v>0.6809999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0.68099999999999994</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
-        <v>45519.8456827662</v>
+        <v>45488</v>
       </c>
       <c r="B6" s="2">
-        <v>45519.8456827662</v>
+        <v>45519.845682766201</v>
       </c>
       <c r="C6" s="3">
         <v>129102</v>
@@ -557,12 +769,15 @@
         <v>2441</v>
       </c>
       <c r="I6" s="4">
-        <v>0.649</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
-        <v>45519.84611283565</v>
+        <v>45488</v>
       </c>
       <c r="B7" s="2">
         <v>45519.84611283565</v>
@@ -588,13 +803,16 @@
       <c r="I7" s="4">
         <v>0.628</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
-        <v>45519.84811866898</v>
+        <v>45488</v>
       </c>
       <c r="B8" s="2">
-        <v>45519.84811866898</v>
+        <v>45519.848118668982</v>
       </c>
       <c r="C8" s="3">
         <v>339564</v>
@@ -615,15 +833,18 @@
         <v>1029</v>
       </c>
       <c r="I8" s="4">
-        <v>0.6729999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>0.67299999999999993</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
-        <v>45519.84845379629</v>
+        <v>45488</v>
       </c>
       <c r="B9" s="2">
-        <v>45519.84845379629</v>
+        <v>45519.848453796287</v>
       </c>
       <c r="C9" s="3">
         <v>368519</v>
@@ -644,15 +865,18 @@
         <v>1664</v>
       </c>
       <c r="I9" s="4">
-        <v>0.662</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
-        <v>45519.84871871528</v>
+        <v>45488</v>
       </c>
       <c r="B10" s="2">
-        <v>45519.84871871528</v>
+        <v>45519.848718715279</v>
       </c>
       <c r="C10" s="3">
         <v>391408</v>
@@ -673,12 +897,15 @@
         <v>1816</v>
       </c>
       <c r="I10" s="4">
-        <v>0.647</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
-        <v>45519.84909113426</v>
+        <v>45488</v>
       </c>
       <c r="B11" s="2">
         <v>45519.84909113426</v>
@@ -702,15 +929,18 @@
         <v>1974</v>
       </c>
       <c r="I11" s="4">
-        <v>0.614</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
-        <v>45519.8494056713</v>
+        <v>45488</v>
       </c>
       <c r="B12" s="2">
-        <v>45519.8494056713</v>
+        <v>45519.849405671303</v>
       </c>
       <c r="C12" s="3">
         <v>450761</v>
@@ -731,12 +961,15 @@
         <v>2269</v>
       </c>
       <c r="I12" s="4">
-        <v>0.646</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="J12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
-        <v>45519.8498209838</v>
+        <v>45488</v>
       </c>
       <c r="B13" s="2">
         <v>45519.8498209838</v>
@@ -760,15 +993,18 @@
         <v>1804</v>
       </c>
       <c r="I13" s="4">
-        <v>0.6719999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>0.67199999999999993</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
-        <v>45519.85010582176</v>
+        <v>45488</v>
       </c>
       <c r="B14" s="2">
-        <v>45519.85010582176</v>
+        <v>45519.850105821759</v>
       </c>
       <c r="C14" s="3">
         <v>511254</v>
@@ -789,12 +1025,15 @@
         <v>1577</v>
       </c>
       <c r="I14" s="4">
-        <v>0.637</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="J14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
-        <v>45519.85046159722</v>
+        <v>45488</v>
       </c>
       <c r="B15" s="2">
         <v>45519.85046159722</v>
@@ -818,15 +1057,18 @@
         <v>1416</v>
       </c>
       <c r="I15" s="4">
-        <v>0.649</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
-        <v>45519.85093976852</v>
+        <v>45488</v>
       </c>
       <c r="B16" s="2">
-        <v>45519.85093976852</v>
+        <v>45519.850939768519</v>
       </c>
       <c r="C16" s="3">
         <v>583307</v>
@@ -847,15 +1089,18 @@
         <v>1253</v>
       </c>
       <c r="I16" s="4">
-        <v>0.667</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
-        <v>45519.8514116088</v>
+        <v>45488</v>
       </c>
       <c r="B17" s="2">
-        <v>45519.8514116088</v>
+        <v>45519.851411608797</v>
       </c>
       <c r="C17" s="3">
         <v>624074</v>
@@ -878,13 +1123,16 @@
       <c r="I17" s="4">
         <v>0.627</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
-        <v>45519.8520075</v>
+        <v>45488</v>
       </c>
       <c r="B18" s="2">
-        <v>45519.8520075</v>
+        <v>45519.852007499998</v>
       </c>
       <c r="C18" s="3">
         <v>675559</v>
@@ -905,15 +1153,18 @@
         <v>2354</v>
       </c>
       <c r="I18" s="4">
-        <v>0.651</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="J18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
-        <v>45519.8522195949</v>
+        <v>45488</v>
       </c>
       <c r="B19" s="2">
-        <v>45519.8522195949</v>
+        <v>45519.852219594897</v>
       </c>
       <c r="C19" s="3">
         <v>693884</v>
@@ -934,15 +1185,18 @@
         <v>1468</v>
       </c>
       <c r="I19" s="4">
-        <v>0.666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
-        <v>45519.85245630787</v>
+        <v>45488</v>
       </c>
       <c r="B20" s="2">
-        <v>45519.85245630787</v>
+        <v>45519.852456307868</v>
       </c>
       <c r="C20" s="3">
         <v>714336</v>
@@ -963,15 +1217,18 @@
         <v>2128</v>
       </c>
       <c r="I20" s="4">
-        <v>0.649</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="J20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
-        <v>45519.85269021991</v>
+        <v>45488</v>
       </c>
       <c r="B21" s="2">
-        <v>45519.85269021991</v>
+        <v>45519.852690219908</v>
       </c>
       <c r="C21" s="3">
         <v>734546</v>
@@ -992,12 +1249,15 @@
         <v>1369</v>
       </c>
       <c r="I21" s="4">
-        <v>0.663</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
-        <v>45519.85291883102</v>
+        <v>45488</v>
       </c>
       <c r="B22" s="2">
         <v>45519.85291883102</v>
@@ -1021,15 +1281,18 @@
         <v>2238</v>
       </c>
       <c r="I22" s="4">
-        <v>0.665</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="J22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
-        <v>45519.85352918982</v>
+        <v>45488</v>
       </c>
       <c r="B23" s="2">
-        <v>45519.85352918982</v>
+        <v>45519.853529189822</v>
       </c>
       <c r="C23" s="3">
         <v>807033</v>
@@ -1052,13 +1315,16 @@
       <c r="I23" s="4">
         <v>0.626</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="J23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
-        <v>45519.85379472222</v>
+        <v>45488</v>
       </c>
       <c r="B24" s="2">
-        <v>45519.85379472222</v>
+        <v>45519.853794722221</v>
       </c>
       <c r="C24" s="3">
         <v>829975</v>
@@ -1079,15 +1345,18 @@
         <v>2203</v>
       </c>
       <c r="I24" s="4">
-        <v>0.614</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="J24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
-        <v>45519.85415224537</v>
+        <v>45488</v>
       </c>
       <c r="B25" s="2">
-        <v>45519.85415224537</v>
+        <v>45519.854152245367</v>
       </c>
       <c r="C25" s="3">
         <v>860865</v>
@@ -1108,15 +1377,18 @@
         <v>1822</v>
       </c>
       <c r="I25" s="4">
-        <v>0.618</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="J25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
-        <v>45519.85443090278</v>
+        <v>45488</v>
       </c>
       <c r="B26" s="2">
-        <v>45519.85443090278</v>
+        <v>45519.854430902778</v>
       </c>
       <c r="C26" s="3">
         <v>884941</v>
@@ -1137,15 +1409,18 @@
         <v>1315</v>
       </c>
       <c r="I26" s="4">
-        <v>0.641</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="J26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
-        <v>45519.85470040509</v>
+        <v>45488</v>
       </c>
       <c r="B27" s="2">
-        <v>45519.85470040509</v>
+        <v>45519.854700405092</v>
       </c>
       <c r="C27" s="3">
         <v>908226</v>
@@ -1166,15 +1441,18 @@
         <v>694</v>
       </c>
       <c r="I27" s="4">
-        <v>0.654</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="J27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
-        <v>45519.85524116898</v>
+        <v>45488</v>
       </c>
       <c r="B28" s="2">
-        <v>45519.85524116898</v>
+        <v>45519.855241168982</v>
       </c>
       <c r="C28" s="3">
         <v>954948</v>
@@ -1195,15 +1473,18 @@
         <v>727</v>
       </c>
       <c r="I28" s="4">
-        <v>0.641</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="J28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
-        <v>45519.85547622685</v>
+        <v>45488</v>
       </c>
       <c r="B29" s="2">
-        <v>45519.85547622685</v>
+        <v>45519.855476226847</v>
       </c>
       <c r="C29" s="3">
         <v>975257</v>
@@ -1224,15 +1505,18 @@
         <v>897</v>
       </c>
       <c r="I29" s="4">
-        <v>0.6739999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>0.67399999999999993</v>
+      </c>
+      <c r="J29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
-        <v>45519.85587212963</v>
+        <v>45488</v>
       </c>
       <c r="B30" s="2">
-        <v>45519.85587212963</v>
+        <v>45519.855872129629</v>
       </c>
       <c r="C30" s="3">
         <v>1009463</v>
@@ -1253,15 +1537,18 @@
         <v>2080</v>
       </c>
       <c r="I30" s="4">
-        <v>0.667</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
-        <v>45519.85610515047</v>
+        <v>45488</v>
       </c>
       <c r="B31" s="2">
-        <v>45519.85610515047</v>
+        <v>45519.856105150473</v>
       </c>
       <c r="C31" s="3">
         <v>1029596</v>
@@ -1282,15 +1569,18 @@
         <v>2536</v>
       </c>
       <c r="I31" s="4">
-        <v>0.633</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="J31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
-        <v>45519.85649165509</v>
+        <v>45488</v>
       </c>
       <c r="B32" s="2">
-        <v>45519.85649165509</v>
+        <v>45519.856491655089</v>
       </c>
       <c r="C32" s="3">
         <v>1062990</v>
@@ -1311,15 +1601,18 @@
         <v>2099</v>
       </c>
       <c r="I32" s="4">
-        <v>0.661</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="J32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
-        <v>45519.85837368055</v>
+        <v>45488</v>
       </c>
       <c r="B33" s="2">
-        <v>45519.85837368055</v>
+        <v>45519.858373680552</v>
       </c>
       <c r="C33" s="3">
         <v>1225597</v>
@@ -1342,13 +1635,16 @@
       <c r="I33" s="4">
         <v>0.623</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
-        <v>45519.85866332176</v>
+        <v>45488</v>
       </c>
       <c r="B34" s="2">
-        <v>45519.85866332176</v>
+        <v>45519.858663321756</v>
       </c>
       <c r="C34" s="3">
         <v>1250622</v>
@@ -1369,15 +1665,18 @@
         <v>926</v>
       </c>
       <c r="I34" s="4">
-        <v>0.652</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="J34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
-        <v>45519.85893459491</v>
+        <v>45488</v>
       </c>
       <c r="B35" s="2">
-        <v>45519.85893459491</v>
+        <v>45519.858934594908</v>
       </c>
       <c r="C35" s="3">
         <v>1274060</v>
@@ -1400,13 +1699,16 @@
       <c r="I35" s="4">
         <v>0.622</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="J35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
-        <v>45519.85921443287</v>
+        <v>45488</v>
       </c>
       <c r="B36" s="2">
-        <v>45519.85921443287</v>
+        <v>45519.859214432872</v>
       </c>
       <c r="C36" s="3">
         <v>1298238</v>
@@ -1427,12 +1729,15 @@
         <v>1794</v>
       </c>
       <c r="I36" s="4">
-        <v>0.654</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="J36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
-        <v>45519.85945408565</v>
+        <v>45488</v>
       </c>
       <c r="B37" s="2">
         <v>45519.85945408565</v>
@@ -1456,15 +1761,18 @@
         <v>1351</v>
       </c>
       <c r="I37" s="4">
-        <v>0.658</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="J37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
-        <v>45519.86009604167</v>
+        <v>45488</v>
       </c>
       <c r="B38" s="2">
-        <v>45519.86009604167</v>
+        <v>45519.860096041673</v>
       </c>
       <c r="C38" s="3">
         <v>1374409</v>
@@ -1487,13 +1795,16 @@
       <c r="I38" s="4">
         <v>0.622</v>
       </c>
-    </row>
-    <row r="39" spans="1:9">
+      <c r="J38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
-        <v>45519.86043104166</v>
+        <v>45488</v>
       </c>
       <c r="B39" s="2">
-        <v>45519.86043104166</v>
+        <v>45519.860431041663</v>
       </c>
       <c r="C39" s="3">
         <v>1403353</v>
@@ -1514,15 +1825,18 @@
         <v>2190</v>
       </c>
       <c r="I39" s="4">
-        <v>0.591</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="J39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
-        <v>45519.86083375</v>
+        <v>45488</v>
       </c>
       <c r="B40" s="2">
-        <v>45519.86083375</v>
+        <v>45519.860833749997</v>
       </c>
       <c r="C40" s="3">
         <v>1438147</v>
@@ -1543,15 +1857,18 @@
         <v>1004</v>
       </c>
       <c r="I40" s="4">
-        <v>0.642</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="J40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
-        <v>45519.86109537037</v>
+        <v>45488</v>
       </c>
       <c r="B41" s="2">
-        <v>45519.86109537037</v>
+        <v>45519.861095370368</v>
       </c>
       <c r="C41" s="3">
         <v>1460751</v>
@@ -1572,15 +1889,18 @@
         <v>2084</v>
       </c>
       <c r="I41" s="4">
-        <v>0.7889999999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>0.78899999999999992</v>
+      </c>
+      <c r="J41" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
-        <v>45519.86135800926</v>
+        <v>45488</v>
       </c>
       <c r="B42" s="2">
-        <v>45519.86135800926</v>
+        <v>45519.861358009257</v>
       </c>
       <c r="C42" s="3">
         <v>1483443</v>
@@ -1601,15 +1921,18 @@
         <v>1013</v>
       </c>
       <c r="I42" s="4">
-        <v>0.637</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="J42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
-        <v>45519.86213372685</v>
+        <v>45488</v>
       </c>
       <c r="B43" s="2">
-        <v>45519.86213372685</v>
+        <v>45519.862133726849</v>
       </c>
       <c r="C43" s="3">
         <v>1550465</v>
@@ -1630,15 +1953,18 @@
         <v>790</v>
       </c>
       <c r="I43" s="4">
-        <v>0.659</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="J43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
-        <v>45519.86237907408</v>
+        <v>45488</v>
       </c>
       <c r="B44" s="2">
-        <v>45519.86237907408</v>
+        <v>45519.862379074082</v>
       </c>
       <c r="C44" s="3">
         <v>1571663</v>
@@ -1659,15 +1985,18 @@
         <v>1648</v>
       </c>
       <c r="I44" s="4">
-        <v>0.631</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="J44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
-        <v>45519.86269222223</v>
+        <v>45488</v>
       </c>
       <c r="B45" s="2">
-        <v>45519.86269222223</v>
+        <v>45519.862692222232</v>
       </c>
       <c r="C45" s="3">
         <v>1598719</v>
@@ -1688,15 +2017,18 @@
         <v>1390</v>
       </c>
       <c r="I45" s="4">
-        <v>0.657</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="J45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
-        <v>45519.86294815972</v>
+        <v>45488</v>
       </c>
       <c r="B46" s="2">
-        <v>45519.86294815972</v>
+        <v>45519.862948159724</v>
       </c>
       <c r="C46" s="3">
         <v>1620832</v>
@@ -1717,15 +2049,18 @@
         <v>1753</v>
       </c>
       <c r="I46" s="4">
-        <v>0.645</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="J46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
-        <v>45519.86335030093</v>
+        <v>45488</v>
       </c>
       <c r="B47" s="2">
-        <v>45519.86335030093</v>
+        <v>45519.863350300933</v>
       </c>
       <c r="C47" s="3">
         <v>1655577</v>
@@ -1748,13 +2083,16 @@
       <c r="I47" s="4">
         <v>0.66</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
+      <c r="J47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
-        <v>45519.86420149305</v>
+        <v>45488</v>
       </c>
       <c r="B48" s="2">
-        <v>45519.86420149305</v>
+        <v>45519.864201493052</v>
       </c>
       <c r="C48" s="3">
         <v>1729120</v>
@@ -1777,13 +2115,16 @@
       <c r="I48" s="4">
         <v>0.626</v>
       </c>
-    </row>
-    <row r="49" spans="1:9">
+      <c r="J48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
-        <v>45519.86443811343</v>
+        <v>45488</v>
       </c>
       <c r="B49" s="2">
-        <v>45519.86443811343</v>
+        <v>45519.864438113429</v>
       </c>
       <c r="C49" s="3">
         <v>1749564</v>
@@ -1804,15 +2145,18 @@
         <v>759</v>
       </c>
       <c r="I49" s="4">
-        <v>0.651</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="J49" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
-        <v>45519.86478012732</v>
+        <v>45488</v>
       </c>
       <c r="B50" s="2">
-        <v>45519.86478012732</v>
+        <v>45519.864780127318</v>
       </c>
       <c r="C50" s="3">
         <v>1779114</v>
@@ -1835,13 +2179,16 @@
       <c r="I50" s="4">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
-        <v>45519.86500248843</v>
+        <v>45488</v>
       </c>
       <c r="B51" s="2">
-        <v>45519.86500248843</v>
+        <v>45519.865002488426</v>
       </c>
       <c r="C51" s="3">
         <v>1798326</v>
@@ -1862,15 +2209,18 @@
         <v>1006</v>
       </c>
       <c r="I51" s="4">
-        <v>0.649</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="J51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
-        <v>45519.86521170139</v>
+        <v>45488</v>
       </c>
       <c r="B52" s="2">
-        <v>45519.86521170139</v>
+        <v>45519.865211701392</v>
       </c>
       <c r="C52" s="3">
         <v>1816402</v>
@@ -1891,15 +2241,18 @@
         <v>1845</v>
       </c>
       <c r="I52" s="4">
-        <v>0.648</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="J52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
-        <v>45519.86593309028</v>
+        <v>45488</v>
       </c>
       <c r="B53" s="2">
-        <v>45519.86593309028</v>
+        <v>45519.865933090281</v>
       </c>
       <c r="C53" s="3">
         <v>1878730</v>
@@ -1922,13 +2275,16 @@
       <c r="I53" s="4">
         <v>0.622</v>
       </c>
-    </row>
-    <row r="54" spans="1:9">
+      <c r="J53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
-        <v>45519.86636268519</v>
+        <v>45488</v>
       </c>
       <c r="B54" s="2">
-        <v>45519.86636268519</v>
+        <v>45519.866362685192</v>
       </c>
       <c r="C54" s="3">
         <v>1915847</v>
@@ -1949,15 +2305,18 @@
         <v>1566</v>
       </c>
       <c r="I54" s="4">
-        <v>0.549</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="J54" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
-        <v>45519.86697696759</v>
+        <v>45488</v>
       </c>
       <c r="B55" s="2">
-        <v>45519.86697696759</v>
+        <v>45519.866976967591</v>
       </c>
       <c r="C55" s="3">
         <v>1968921</v>
@@ -1978,15 +2337,18 @@
         <v>734</v>
       </c>
       <c r="I55" s="4">
-        <v>0.649</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="J55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
-        <v>45519.86720634259</v>
+        <v>45488</v>
       </c>
       <c r="B56" s="2">
-        <v>45519.86720634259</v>
+        <v>45519.867206342591</v>
       </c>
       <c r="C56" s="3">
         <v>1988739</v>
@@ -2007,12 +2369,15 @@
         <v>695</v>
       </c>
       <c r="I56" s="4">
-        <v>0.666</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="J56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
-        <v>45519.86744707176</v>
+        <v>45488</v>
       </c>
       <c r="B57" s="2">
         <v>45519.86744707176</v>
@@ -2036,15 +2401,18 @@
         <v>2883</v>
       </c>
       <c r="I57" s="4">
-        <v>0.647</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="J57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
-        <v>45519.86780920139</v>
+        <v>45488</v>
       </c>
       <c r="B58" s="2">
-        <v>45519.86780920139</v>
+        <v>45519.867809201387</v>
       </c>
       <c r="C58" s="3">
         <v>2040826</v>
@@ -2065,15 +2433,18 @@
         <v>957</v>
       </c>
       <c r="I58" s="4">
-        <v>0.659</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="J58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
-        <v>45519.86803394676</v>
+        <v>45488</v>
       </c>
       <c r="B59" s="2">
-        <v>45519.86803394676</v>
+        <v>45519.868033946761</v>
       </c>
       <c r="C59" s="3">
         <v>2060244</v>
@@ -2094,15 +2465,18 @@
         <v>279</v>
       </c>
       <c r="I59" s="4">
-        <v>0.756</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="J59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
-        <v>45519.86830049769</v>
+        <v>45488</v>
       </c>
       <c r="B60" s="2">
-        <v>45519.86830049769</v>
+        <v>45519.868300497692</v>
       </c>
       <c r="C60" s="3">
         <v>2083274</v>
@@ -2123,15 +2497,18 @@
         <v>939</v>
       </c>
       <c r="I60" s="4">
-        <v>0.609</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="J60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
-        <v>45519.86867112268</v>
+        <v>45488</v>
       </c>
       <c r="B61" s="2">
-        <v>45519.86867112268</v>
+        <v>45519.868671122676</v>
       </c>
       <c r="C61" s="3">
         <v>2115296</v>
@@ -2154,13 +2531,16 @@
       <c r="I61" s="4">
         <v>0.626</v>
       </c>
-    </row>
-    <row r="62" spans="1:9">
+      <c r="J61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
-        <v>45519.86902512732</v>
+        <v>45488</v>
       </c>
       <c r="B62" s="2">
-        <v>45519.86902512732</v>
+        <v>45519.869025127322</v>
       </c>
       <c r="C62" s="3">
         <v>2145882</v>
@@ -2181,7 +2561,10 @@
         <v>1149</v>
       </c>
       <c r="I62" s="4">
-        <v>0.643</v>
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="J62" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>